<commit_message>
update Git to JAM XL
see title
</commit_message>
<xml_diff>
--- a/docs/Norman_JAM_to_Git_Inventory.xlsx
+++ b/docs/Norman_JAM_to_Git_Inventory.xlsx
@@ -1721,7 +1721,7 @@
   <dimension ref="A1:L391"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H246" sqref="H246:H247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4903,7 +4903,7 @@
         <v>274</v>
       </c>
       <c r="H229" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
@@ -4914,7 +4914,7 @@
         <v>275</v>
       </c>
       <c r="H230" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
@@ -4925,7 +4925,7 @@
         <v>276</v>
       </c>
       <c r="H231" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
@@ -4936,7 +4936,7 @@
         <v>277</v>
       </c>
       <c r="H232" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
@@ -4947,7 +4947,7 @@
         <v>278</v>
       </c>
       <c r="H233" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
@@ -4958,7 +4958,7 @@
         <v>279</v>
       </c>
       <c r="H234" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
@@ -4969,7 +4969,7 @@
         <v>280</v>
       </c>
       <c r="H235" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
@@ -4980,7 +4980,7 @@
         <v>281</v>
       </c>
       <c r="H236" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
@@ -4991,7 +4991,7 @@
         <v>282</v>
       </c>
       <c r="H237" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
@@ -5002,7 +5002,7 @@
         <v>283</v>
       </c>
       <c r="H238" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
@@ -5013,7 +5013,7 @@
         <v>284</v>
       </c>
       <c r="H239" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
@@ -5024,7 +5024,7 @@
         <v>285</v>
       </c>
       <c r="H240" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
@@ -5035,7 +5035,7 @@
         <v>286</v>
       </c>
       <c r="H241" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>287</v>
       </c>
       <c r="H242" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
@@ -5057,7 +5057,7 @@
         <v>288</v>
       </c>
       <c r="H243" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
@@ -5068,7 +5068,7 @@
         <v>289</v>
       </c>
       <c r="H244" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
@@ -5087,7 +5087,7 @@
         <v>290</v>
       </c>
       <c r="H246" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
@@ -5098,7 +5098,7 @@
         <v>291</v>
       </c>
       <c r="H247" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated xl about porting doc's from jam to git wiki
see title
</commit_message>
<xml_diff>
--- a/docs/Norman_JAM_to_Git_Inventory.xlsx
+++ b/docs/Norman_JAM_to_Git_Inventory.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I311750\Documents\GitHub\Norman\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="19440" windowHeight="11040"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="444">
   <si>
     <t>Content</t>
   </si>
@@ -1302,9 +1307,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>yes (first two columns only)</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -1348,6 +1350,9 @@
   </si>
   <si>
     <t>decision pending - Nir</t>
+  </si>
+  <si>
+    <t>https://github.wdf.sap.corp/Norman/Norman/tree/master/docs/QA/Testing%20Tool%20Guides/Mocha</t>
   </si>
 </sst>
 </file>
@@ -1427,6 +1432,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1474,7 +1482,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1509,7 +1517,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1720,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H246" sqref="H246:H247"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,16 +1746,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>425</v>
@@ -1780,13 +1788,13 @@
         <v>427</v>
       </c>
       <c r="I3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1801,13 +1809,13 @@
         <v>427</v>
       </c>
       <c r="I4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1822,13 +1830,13 @@
         <v>427</v>
       </c>
       <c r="I5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1843,13 +1851,13 @@
         <v>427</v>
       </c>
       <c r="I6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1864,13 +1872,13 @@
         <v>427</v>
       </c>
       <c r="I7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1885,13 +1893,13 @@
         <v>427</v>
       </c>
       <c r="I8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1906,13 +1914,13 @@
         <v>427</v>
       </c>
       <c r="I9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1927,13 +1935,13 @@
         <v>427</v>
       </c>
       <c r="I10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1948,13 +1956,13 @@
         <v>427</v>
       </c>
       <c r="I11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1969,13 +1977,13 @@
         <v>427</v>
       </c>
       <c r="I12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1990,13 +1998,13 @@
         <v>427</v>
       </c>
       <c r="I13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2011,13 +2019,13 @@
         <v>427</v>
       </c>
       <c r="I14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2032,13 +2040,13 @@
         <v>427</v>
       </c>
       <c r="I15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2053,13 +2061,13 @@
         <v>427</v>
       </c>
       <c r="I16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K16" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2074,13 +2082,13 @@
         <v>427</v>
       </c>
       <c r="I17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2095,13 +2103,13 @@
         <v>427</v>
       </c>
       <c r="I18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K18" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2116,13 +2124,13 @@
         <v>427</v>
       </c>
       <c r="I19" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K19" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2137,13 +2145,13 @@
         <v>427</v>
       </c>
       <c r="I20" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2158,13 +2166,13 @@
         <v>427</v>
       </c>
       <c r="I21" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2179,13 +2187,13 @@
         <v>427</v>
       </c>
       <c r="I22" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K22" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2200,13 +2208,13 @@
         <v>427</v>
       </c>
       <c r="I23" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K23" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2221,13 +2229,13 @@
         <v>427</v>
       </c>
       <c r="I24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K24" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2242,13 +2250,13 @@
         <v>427</v>
       </c>
       <c r="I25" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K25" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2263,13 +2271,13 @@
         <v>427</v>
       </c>
       <c r="I26" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K26" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2284,13 +2292,13 @@
         <v>427</v>
       </c>
       <c r="I27" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K27" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2305,13 +2313,13 @@
         <v>427</v>
       </c>
       <c r="I28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2326,13 +2334,13 @@
         <v>427</v>
       </c>
       <c r="I29" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2347,13 +2355,13 @@
         <v>427</v>
       </c>
       <c r="I30" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K30" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2368,13 +2376,13 @@
         <v>427</v>
       </c>
       <c r="I31" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K31" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2389,13 +2397,13 @@
         <v>427</v>
       </c>
       <c r="I32" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K32" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2410,13 +2418,13 @@
         <v>427</v>
       </c>
       <c r="I33" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K33" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2431,13 +2439,13 @@
         <v>427</v>
       </c>
       <c r="I34" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K34" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2452,13 +2460,13 @@
         <v>427</v>
       </c>
       <c r="I35" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K35" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2473,13 +2481,13 @@
         <v>427</v>
       </c>
       <c r="I36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K36" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2494,13 +2502,13 @@
         <v>427</v>
       </c>
       <c r="I37" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K37" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2515,13 +2523,13 @@
         <v>427</v>
       </c>
       <c r="I38" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2536,13 +2544,13 @@
         <v>427</v>
       </c>
       <c r="I39" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2557,13 +2565,13 @@
         <v>427</v>
       </c>
       <c r="I40" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K40" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2580,13 +2588,13 @@
         <v>427</v>
       </c>
       <c r="I41" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J41" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K41" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2601,13 +2609,13 @@
         <v>427</v>
       </c>
       <c r="I42" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J42" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K42" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2622,13 +2630,13 @@
         <v>427</v>
       </c>
       <c r="I43" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K43" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2643,13 +2651,13 @@
         <v>427</v>
       </c>
       <c r="I44" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K44" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2664,13 +2672,13 @@
         <v>427</v>
       </c>
       <c r="I45" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K45" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2685,13 +2693,13 @@
         <v>427</v>
       </c>
       <c r="I46" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K46" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2706,13 +2714,13 @@
         <v>427</v>
       </c>
       <c r="I47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K47" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2727,13 +2735,13 @@
         <v>427</v>
       </c>
       <c r="I48" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -2748,13 +2756,13 @@
         <v>427</v>
       </c>
       <c r="I49" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J49" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K49" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2769,13 +2777,13 @@
         <v>427</v>
       </c>
       <c r="I50" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J50" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2790,13 +2798,13 @@
         <v>427</v>
       </c>
       <c r="I51" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K51" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2811,13 +2819,13 @@
         <v>427</v>
       </c>
       <c r="I52" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J52" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="K52" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2834,10 +2842,10 @@
         <v>427</v>
       </c>
       <c r="I53" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K53" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2852,10 +2860,10 @@
         <v>427</v>
       </c>
       <c r="I54" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K54" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2872,13 +2880,13 @@
         <v>427</v>
       </c>
       <c r="I55" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J55" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K55" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2893,13 +2901,13 @@
         <v>427</v>
       </c>
       <c r="I56" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J56" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K56" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -2914,13 +2922,13 @@
         <v>427</v>
       </c>
       <c r="I57" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J57" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K57" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -3568,10 +3576,10 @@
         <v>427</v>
       </c>
       <c r="I111" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J111" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -3585,10 +3593,10 @@
         <v>427</v>
       </c>
       <c r="I112" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J112" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -3599,7 +3607,7 @@
         <v>194</v>
       </c>
       <c r="H113" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -3610,7 +3618,7 @@
         <v>195</v>
       </c>
       <c r="H114" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -3621,7 +3629,7 @@
         <v>193</v>
       </c>
       <c r="H115" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -3632,7 +3640,7 @@
         <v>196</v>
       </c>
       <c r="H116" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -3643,7 +3651,7 @@
         <v>193</v>
       </c>
       <c r="H117" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -3654,7 +3662,7 @@
         <v>193</v>
       </c>
       <c r="H118" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -3665,7 +3673,7 @@
         <v>197</v>
       </c>
       <c r="H119" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -3676,7 +3684,7 @@
         <v>198</v>
       </c>
       <c r="H120" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3687,7 +3695,7 @@
         <v>199</v>
       </c>
       <c r="H121" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -3698,7 +3706,7 @@
         <v>200</v>
       </c>
       <c r="H122" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -3709,7 +3717,7 @@
         <v>201</v>
       </c>
       <c r="H123" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -3720,7 +3728,7 @@
         <v>202</v>
       </c>
       <c r="H124" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -3731,7 +3739,7 @@
         <v>203</v>
       </c>
       <c r="H125" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -3742,7 +3750,7 @@
         <v>204</v>
       </c>
       <c r="H126" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -3753,7 +3761,7 @@
         <v>205</v>
       </c>
       <c r="H127" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -3764,7 +3772,7 @@
         <v>206</v>
       </c>
       <c r="H128" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
@@ -3775,7 +3783,7 @@
         <v>207</v>
       </c>
       <c r="H129" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
@@ -3786,7 +3794,7 @@
         <v>208</v>
       </c>
       <c r="H130" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
@@ -3797,7 +3805,7 @@
         <v>209</v>
       </c>
       <c r="H131" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
@@ -3808,7 +3816,7 @@
         <v>210</v>
       </c>
       <c r="H132" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
@@ -3819,7 +3827,7 @@
         <v>211</v>
       </c>
       <c r="H133" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
@@ -3830,7 +3838,7 @@
         <v>212</v>
       </c>
       <c r="H134" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
@@ -3841,7 +3849,7 @@
         <v>213</v>
       </c>
       <c r="H135" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
@@ -3862,7 +3870,7 @@
         <v>214</v>
       </c>
       <c r="H137" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J137" t="s">
         <v>426</v>
@@ -3876,7 +3884,7 @@
         <v>215</v>
       </c>
       <c r="H138" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
@@ -3887,7 +3895,7 @@
         <v>216</v>
       </c>
       <c r="H139" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
@@ -3898,7 +3906,7 @@
         <v>217</v>
       </c>
       <c r="H140" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
@@ -3909,7 +3917,7 @@
         <v>218</v>
       </c>
       <c r="H141" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
@@ -3920,7 +3928,7 @@
         <v>219</v>
       </c>
       <c r="H142" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
@@ -3931,7 +3939,7 @@
         <v>220</v>
       </c>
       <c r="H143" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
@@ -3942,7 +3950,7 @@
         <v>221</v>
       </c>
       <c r="H144" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -3953,7 +3961,7 @@
         <v>222</v>
       </c>
       <c r="H145" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -3964,7 +3972,7 @@
         <v>223</v>
       </c>
       <c r="H146" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -3975,7 +3983,7 @@
         <v>224</v>
       </c>
       <c r="H147" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -3986,7 +3994,7 @@
         <v>225</v>
       </c>
       <c r="H148" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -4005,7 +4013,7 @@
         <v>226</v>
       </c>
       <c r="H150" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -4016,7 +4024,7 @@
         <v>227</v>
       </c>
       <c r="H151" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -4027,7 +4035,7 @@
         <v>228</v>
       </c>
       <c r="H152" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -4038,7 +4046,7 @@
         <v>229</v>
       </c>
       <c r="H153" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -4049,7 +4057,7 @@
         <v>230</v>
       </c>
       <c r="H154" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -4060,7 +4068,7 @@
         <v>231</v>
       </c>
       <c r="H155" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -4071,7 +4079,7 @@
         <v>232</v>
       </c>
       <c r="H156" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -4090,7 +4098,7 @@
         <v>233</v>
       </c>
       <c r="H158" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -4101,7 +4109,7 @@
         <v>234</v>
       </c>
       <c r="H159" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -4112,7 +4120,7 @@
         <v>238</v>
       </c>
       <c r="H160" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
@@ -4123,7 +4131,7 @@
         <v>235</v>
       </c>
       <c r="H161" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
@@ -4134,7 +4142,7 @@
         <v>236</v>
       </c>
       <c r="H162" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
@@ -4145,7 +4153,7 @@
         <v>237</v>
       </c>
       <c r="H163" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
@@ -4158,7 +4166,7 @@
         <v>239</v>
       </c>
       <c r="H164" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
@@ -4177,7 +4185,7 @@
         <v>240</v>
       </c>
       <c r="H166" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
@@ -4188,7 +4196,7 @@
         <v>241</v>
       </c>
       <c r="H167" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
@@ -4199,7 +4207,7 @@
         <v>242</v>
       </c>
       <c r="H168" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
@@ -4210,7 +4218,7 @@
         <v>243</v>
       </c>
       <c r="H169" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
@@ -4236,8 +4244,11 @@
       <c r="H171" t="s">
         <v>427</v>
       </c>
+      <c r="I171" t="s">
+        <v>429</v>
+      </c>
       <c r="J171" t="s">
-        <v>427</v>
+        <v>443</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
@@ -4251,6 +4262,12 @@
       <c r="H172" t="s">
         <v>427</v>
       </c>
+      <c r="I172" t="s">
+        <v>429</v>
+      </c>
+      <c r="J172" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
@@ -4263,6 +4280,12 @@
       <c r="H173" t="s">
         <v>427</v>
       </c>
+      <c r="I173" t="s">
+        <v>429</v>
+      </c>
+      <c r="J173" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
@@ -4275,6 +4298,12 @@
       <c r="H174" t="s">
         <v>427</v>
       </c>
+      <c r="I174" t="s">
+        <v>429</v>
+      </c>
+      <c r="J174" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
@@ -4287,6 +4316,12 @@
       <c r="H175" t="s">
         <v>427</v>
       </c>
+      <c r="I175" t="s">
+        <v>429</v>
+      </c>
+      <c r="J175" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
@@ -4299,8 +4334,14 @@
       <c r="H176" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I176" t="s">
+        <v>429</v>
+      </c>
+      <c r="J176" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4311,8 +4352,14 @@
       <c r="H177" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I177" t="s">
+        <v>429</v>
+      </c>
+      <c r="J177" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4323,8 +4370,14 @@
       <c r="H178" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I178" t="s">
+        <v>429</v>
+      </c>
+      <c r="J178" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="2" t="s">
@@ -4332,7 +4385,7 @@
       </c>
       <c r="D179" s="1"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="2"/>
@@ -4342,8 +4395,14 @@
       <c r="H180" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I180" t="s">
+        <v>429</v>
+      </c>
+      <c r="J180" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="2"/>
@@ -4353,8 +4412,14 @@
       <c r="H181" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I181" t="s">
+        <v>429</v>
+      </c>
+      <c r="J181" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1" t="s">
         <v>20</v>
@@ -4369,7 +4434,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1" t="s">
@@ -4379,7 +4444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="2" t="s">
@@ -4389,10 +4454,10 @@
         <v>254</v>
       </c>
       <c r="H184" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1" t="s">
@@ -4400,7 +4465,7 @@
       </c>
       <c r="D185" s="1"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4408,10 +4473,10 @@
         <v>255</v>
       </c>
       <c r="H186" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4419,10 +4484,10 @@
         <v>256</v>
       </c>
       <c r="H187" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4430,10 +4495,10 @@
         <v>257</v>
       </c>
       <c r="H188" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4441,10 +4506,10 @@
         <v>258</v>
       </c>
       <c r="H189" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4452,10 +4517,10 @@
         <v>259</v>
       </c>
       <c r="H190" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4463,10 +4528,10 @@
         <v>260</v>
       </c>
       <c r="H191" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4474,7 +4539,7 @@
         <v>261</v>
       </c>
       <c r="H192" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -4490,7 +4555,7 @@
         <v>262</v>
       </c>
       <c r="H193" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -4509,7 +4574,7 @@
         <v>263</v>
       </c>
       <c r="H195" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -4520,7 +4585,7 @@
         <v>264</v>
       </c>
       <c r="H196" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -4531,7 +4596,7 @@
         <v>265</v>
       </c>
       <c r="H197" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
@@ -4544,7 +4609,7 @@
         <v>266</v>
       </c>
       <c r="H198" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -4557,7 +4622,7 @@
         <v>267</v>
       </c>
       <c r="H199" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
@@ -4576,7 +4641,7 @@
         <v>268</v>
       </c>
       <c r="H201" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
@@ -4587,7 +4652,7 @@
         <v>269</v>
       </c>
       <c r="H202" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
@@ -4598,7 +4663,7 @@
         <v>270</v>
       </c>
       <c r="H203" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
@@ -4609,7 +4674,7 @@
         <v>271</v>
       </c>
       <c r="H204" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
@@ -4622,7 +4687,7 @@
       </c>
       <c r="D205" s="1"/>
       <c r="H205" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
@@ -4633,7 +4698,7 @@
       </c>
       <c r="D206" s="1"/>
       <c r="H206" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
@@ -4644,7 +4709,7 @@
       </c>
       <c r="D207" s="1"/>
       <c r="H207" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
@@ -4666,7 +4731,7 @@
         <v>317</v>
       </c>
       <c r="H209" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
@@ -4678,7 +4743,7 @@
         <v>318</v>
       </c>
       <c r="H210" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
@@ -4692,7 +4757,7 @@
         <v>319</v>
       </c>
       <c r="H211" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -4704,7 +4769,7 @@
         <v>320</v>
       </c>
       <c r="H212" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -4716,7 +4781,7 @@
         <v>321</v>
       </c>
       <c r="H213" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -4730,7 +4795,7 @@
         <v>322</v>
       </c>
       <c r="H214" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
@@ -4742,7 +4807,7 @@
         <v>323</v>
       </c>
       <c r="H215" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
@@ -4763,7 +4828,7 @@
         <v>316</v>
       </c>
       <c r="H217" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -4776,7 +4841,7 @@
         <v>324</v>
       </c>
       <c r="H218" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -4789,7 +4854,7 @@
         <v>325</v>
       </c>
       <c r="H219" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -4802,7 +4867,7 @@
         <v>327</v>
       </c>
       <c r="H220" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -4813,7 +4878,7 @@
         <v>328</v>
       </c>
       <c r="H221" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -4834,7 +4899,7 @@
         <v>329</v>
       </c>
       <c r="H223" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -4847,7 +4912,7 @@
         <v>330</v>
       </c>
       <c r="H224" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -4860,7 +4925,7 @@
         <v>331</v>
       </c>
       <c r="H225" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
@@ -4875,7 +4940,7 @@
         <v>29</v>
       </c>
       <c r="H226" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
@@ -4886,7 +4951,7 @@
         <v>30</v>
       </c>
       <c r="H227" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
@@ -4903,7 +4968,7 @@
         <v>274</v>
       </c>
       <c r="H229" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
@@ -4914,7 +4979,7 @@
         <v>275</v>
       </c>
       <c r="H230" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
@@ -4925,7 +4990,7 @@
         <v>276</v>
       </c>
       <c r="H231" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
@@ -4936,7 +5001,7 @@
         <v>277</v>
       </c>
       <c r="H232" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
@@ -4947,7 +5012,7 @@
         <v>278</v>
       </c>
       <c r="H233" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
@@ -4958,7 +5023,7 @@
         <v>279</v>
       </c>
       <c r="H234" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
@@ -4969,7 +5034,7 @@
         <v>280</v>
       </c>
       <c r="H235" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
@@ -4980,7 +5045,7 @@
         <v>281</v>
       </c>
       <c r="H236" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
@@ -4991,7 +5056,7 @@
         <v>282</v>
       </c>
       <c r="H237" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
@@ -5002,7 +5067,7 @@
         <v>283</v>
       </c>
       <c r="H238" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
@@ -5013,7 +5078,7 @@
         <v>284</v>
       </c>
       <c r="H239" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
@@ -5024,7 +5089,7 @@
         <v>285</v>
       </c>
       <c r="H240" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
@@ -5035,7 +5100,7 @@
         <v>286</v>
       </c>
       <c r="H241" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
@@ -5046,7 +5111,7 @@
         <v>287</v>
       </c>
       <c r="H242" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
@@ -5057,7 +5122,7 @@
         <v>288</v>
       </c>
       <c r="H243" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
@@ -5068,7 +5133,7 @@
         <v>289</v>
       </c>
       <c r="H244" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
@@ -5087,7 +5152,7 @@
         <v>290</v>
       </c>
       <c r="H246" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
@@ -5098,7 +5163,7 @@
         <v>291</v>
       </c>
       <c r="H247" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
@@ -5117,7 +5182,7 @@
         <v>292</v>
       </c>
       <c r="H249" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
@@ -5139,7 +5204,7 @@
         <v>294</v>
       </c>
       <c r="H251" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
@@ -5151,7 +5216,7 @@
         <v>295</v>
       </c>
       <c r="H252" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
@@ -5165,7 +5230,7 @@
         <v>297</v>
       </c>
       <c r="H253" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
@@ -5184,7 +5249,7 @@
         <v>272</v>
       </c>
       <c r="H255" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
@@ -5213,7 +5278,7 @@
         <v>35</v>
       </c>
       <c r="H257" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
@@ -5227,7 +5292,7 @@
         <v>36</v>
       </c>
       <c r="H258" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
@@ -5241,7 +5306,7 @@
         <v>37</v>
       </c>
       <c r="H259" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
@@ -5255,7 +5320,7 @@
         <v>38</v>
       </c>
       <c r="H260" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
@@ -5269,7 +5334,7 @@
         <v>39</v>
       </c>
       <c r="H261" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
@@ -5283,7 +5348,7 @@
         <v>40</v>
       </c>
       <c r="H262" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
@@ -5297,7 +5362,7 @@
         <v>41</v>
       </c>
       <c r="H263" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
@@ -5311,7 +5376,7 @@
         <v>42</v>
       </c>
       <c r="H264" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
@@ -5325,7 +5390,7 @@
         <v>43</v>
       </c>
       <c r="H265" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
@@ -5339,7 +5404,7 @@
         <v>44</v>
       </c>
       <c r="H266" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
@@ -5353,7 +5418,7 @@
         <v>45</v>
       </c>
       <c r="H267" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
@@ -5372,7 +5437,7 @@
         <v>298</v>
       </c>
       <c r="H269" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.25">
@@ -5383,7 +5448,7 @@
         <v>299</v>
       </c>
       <c r="H270" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
@@ -5394,7 +5459,7 @@
         <v>300</v>
       </c>
       <c r="H271" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.25">
@@ -5405,7 +5470,7 @@
         <v>301</v>
       </c>
       <c r="H272" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
@@ -5416,7 +5481,7 @@
         <v>302</v>
       </c>
       <c r="H273" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
@@ -5427,7 +5492,7 @@
         <v>303</v>
       </c>
       <c r="H274" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
@@ -5438,7 +5503,7 @@
         <v>304</v>
       </c>
       <c r="H275" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
@@ -5449,7 +5514,7 @@
         <v>305</v>
       </c>
       <c r="H276" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
@@ -5460,7 +5525,7 @@
         <v>306</v>
       </c>
       <c r="H277" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
@@ -5476,7 +5541,7 @@
         <v>307</v>
       </c>
       <c r="H278" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.25">
@@ -5492,7 +5557,7 @@
         <v>308</v>
       </c>
       <c r="H279" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.25">
@@ -5506,7 +5571,7 @@
         <v>309</v>
       </c>
       <c r="H280" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.25">
@@ -5518,7 +5583,7 @@
         <v>310</v>
       </c>
       <c r="H281" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.25">
@@ -5530,7 +5595,7 @@
         <v>311</v>
       </c>
       <c r="H282" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.25">
@@ -5544,7 +5609,7 @@
         <v>312</v>
       </c>
       <c r="H283" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.25">
@@ -5558,7 +5623,7 @@
         <v>313</v>
       </c>
       <c r="H284" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.25">
@@ -5572,7 +5637,7 @@
       </c>
       <c r="E285" s="2"/>
       <c r="H285" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.25">
@@ -5584,7 +5649,7 @@
       </c>
       <c r="E286" s="2"/>
       <c r="H286" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="287" spans="1:8" x14ac:dyDescent="0.25">
@@ -5611,7 +5676,7 @@
         <v>333</v>
       </c>
       <c r="H289" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.25">
@@ -5622,7 +5687,7 @@
         <v>334</v>
       </c>
       <c r="H290" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.25">
@@ -5633,7 +5698,7 @@
         <v>335</v>
       </c>
       <c r="H291" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.25">
@@ -5644,7 +5709,7 @@
         <v>336</v>
       </c>
       <c r="H292" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
@@ -5657,7 +5722,7 @@
         <v>337</v>
       </c>
       <c r="H293" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
@@ -5688,10 +5753,10 @@
         <v>340</v>
       </c>
       <c r="H296" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J296" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.25">
@@ -5703,7 +5768,7 @@
         <v>341</v>
       </c>
       <c r="H297" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.25">
@@ -5715,7 +5780,7 @@
         <v>342</v>
       </c>
       <c r="H298" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.25">
@@ -5727,7 +5792,7 @@
         <v>343</v>
       </c>
       <c r="H299" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.25">
@@ -5739,7 +5804,7 @@
         <v>344</v>
       </c>
       <c r="H300" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
@@ -5751,7 +5816,7 @@
         <v>345</v>
       </c>
       <c r="H301" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.25">
@@ -5763,7 +5828,7 @@
         <v>346</v>
       </c>
       <c r="H302" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.25">
@@ -5775,7 +5840,7 @@
         <v>347</v>
       </c>
       <c r="H303" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
@@ -5787,7 +5852,7 @@
         <v>348</v>
       </c>
       <c r="H304" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.25">
@@ -5799,7 +5864,7 @@
         <v>349</v>
       </c>
       <c r="H305" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.25">
@@ -5811,7 +5876,7 @@
         <v>350</v>
       </c>
       <c r="H306" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.25">
@@ -5823,7 +5888,7 @@
         <v>351</v>
       </c>
       <c r="H307" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.25">
@@ -5835,7 +5900,7 @@
         <v>352</v>
       </c>
       <c r="H308" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.25">
@@ -5847,7 +5912,7 @@
         <v>353</v>
       </c>
       <c r="H309" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.25">
@@ -5859,7 +5924,7 @@
         <v>354</v>
       </c>
       <c r="H310" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.25">
@@ -5871,7 +5936,7 @@
         <v>355</v>
       </c>
       <c r="H311" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.25">
@@ -5883,7 +5948,7 @@
         <v>356</v>
       </c>
       <c r="H312" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.25">
@@ -5895,7 +5960,7 @@
         <v>357</v>
       </c>
       <c r="H313" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.25">
@@ -5907,7 +5972,7 @@
         <v>358</v>
       </c>
       <c r="H314" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.25">
@@ -5919,7 +5984,7 @@
         <v>359</v>
       </c>
       <c r="H315" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.25">
@@ -5933,7 +5998,7 @@
         <v>360</v>
       </c>
       <c r="H316" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.25">
@@ -5945,7 +6010,7 @@
         <v>361</v>
       </c>
       <c r="H317" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="318" spans="1:8" x14ac:dyDescent="0.25">
@@ -5957,7 +6022,7 @@
         <v>362</v>
       </c>
       <c r="H318" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.25">
@@ -5969,7 +6034,7 @@
         <v>363</v>
       </c>
       <c r="H319" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.25">
@@ -5981,7 +6046,7 @@
         <v>364</v>
       </c>
       <c r="H320" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.25">
@@ -5993,7 +6058,7 @@
         <v>365</v>
       </c>
       <c r="H321" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.25">
@@ -6005,7 +6070,7 @@
         <v>366</v>
       </c>
       <c r="H322" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.25">
@@ -6017,7 +6082,7 @@
         <v>367</v>
       </c>
       <c r="H323" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.25">
@@ -6029,7 +6094,7 @@
         <v>368</v>
       </c>
       <c r="H324" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.25">
@@ -6041,7 +6106,7 @@
         <v>369</v>
       </c>
       <c r="H325" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.25">
@@ -6053,7 +6118,7 @@
         <v>370</v>
       </c>
       <c r="H326" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.25">
@@ -6065,7 +6130,7 @@
         <v>371</v>
       </c>
       <c r="H327" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.25">
@@ -6088,7 +6153,7 @@
         <v>25</v>
       </c>
       <c r="H329" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.25">
@@ -6101,7 +6166,7 @@
         <v>72</v>
       </c>
       <c r="H330" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.25">
@@ -6112,7 +6177,7 @@
         <v>73</v>
       </c>
       <c r="H331" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.25">
@@ -6123,7 +6188,7 @@
         <v>50</v>
       </c>
       <c r="H332" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="333" spans="1:8" x14ac:dyDescent="0.25">
@@ -6134,7 +6199,7 @@
         <v>74</v>
       </c>
       <c r="H333" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.25">
@@ -6145,7 +6210,7 @@
         <v>75</v>
       </c>
       <c r="H334" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.25">
@@ -6156,7 +6221,7 @@
         <v>76</v>
       </c>
       <c r="H335" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="336" spans="1:8" x14ac:dyDescent="0.25">
@@ -6167,7 +6232,7 @@
         <v>77</v>
       </c>
       <c r="H336" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.25">
@@ -6197,7 +6262,7 @@
         <v>413</v>
       </c>
       <c r="H339" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="340" spans="1:8" x14ac:dyDescent="0.25">
@@ -6211,7 +6276,7 @@
         <v>414</v>
       </c>
       <c r="H340" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="341" spans="1:8" x14ac:dyDescent="0.25">
@@ -6225,7 +6290,7 @@
         <v>415</v>
       </c>
       <c r="H341" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="342" spans="1:8" x14ac:dyDescent="0.25">
@@ -6237,7 +6302,7 @@
         <v>416</v>
       </c>
       <c r="H342" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="343" spans="1:8" x14ac:dyDescent="0.25">
@@ -6251,7 +6316,7 @@
         <v>417</v>
       </c>
       <c r="H343" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="344" spans="1:8" x14ac:dyDescent="0.25">
@@ -6265,7 +6330,7 @@
         <v>418</v>
       </c>
       <c r="H344" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="345" spans="1:8" x14ac:dyDescent="0.25">
@@ -6300,7 +6365,7 @@
         <v>404</v>
       </c>
       <c r="H348" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="349" spans="1:8" x14ac:dyDescent="0.25">
@@ -6311,7 +6376,7 @@
         <v>178</v>
       </c>
       <c r="H349" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="350" spans="1:8" x14ac:dyDescent="0.25">
@@ -6322,7 +6387,7 @@
         <v>405</v>
       </c>
       <c r="H350" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="351" spans="1:8" x14ac:dyDescent="0.25">
@@ -6333,7 +6398,7 @@
         <v>406</v>
       </c>
       <c r="H351" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="352" spans="1:8" x14ac:dyDescent="0.25">
@@ -6344,7 +6409,7 @@
         <v>407</v>
       </c>
       <c r="H352" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="353" spans="1:8" x14ac:dyDescent="0.25">
@@ -6355,7 +6420,7 @@
         <v>408</v>
       </c>
       <c r="H353" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="354" spans="1:8" x14ac:dyDescent="0.25">
@@ -6366,7 +6431,7 @@
         <v>409</v>
       </c>
       <c r="H354" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="355" spans="1:8" x14ac:dyDescent="0.25">
@@ -6377,7 +6442,7 @@
         <v>410</v>
       </c>
       <c r="H355" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="356" spans="1:8" x14ac:dyDescent="0.25">
@@ -6388,7 +6453,7 @@
         <v>330</v>
       </c>
       <c r="H356" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="357" spans="1:8" x14ac:dyDescent="0.25">
@@ -6407,7 +6472,7 @@
         <v>401</v>
       </c>
       <c r="H358" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="359" spans="1:8" x14ac:dyDescent="0.25">
@@ -6418,7 +6483,7 @@
         <v>402</v>
       </c>
       <c r="H359" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.25">
@@ -6429,7 +6494,7 @@
         <v>403</v>
       </c>
       <c r="H360" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="361" spans="1:8" x14ac:dyDescent="0.25">
@@ -6442,7 +6507,7 @@
         <v>400</v>
       </c>
       <c r="H361" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="362" spans="1:8" x14ac:dyDescent="0.25">
@@ -6457,7 +6522,7 @@
         <v>372</v>
       </c>
       <c r="H362" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="363" spans="1:8" x14ac:dyDescent="0.25">
@@ -6468,7 +6533,7 @@
         <v>373</v>
       </c>
       <c r="H363" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="364" spans="1:8" x14ac:dyDescent="0.25">
@@ -6479,7 +6544,7 @@
         <v>374</v>
       </c>
       <c r="H364" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="365" spans="1:8" x14ac:dyDescent="0.25">
@@ -6490,7 +6555,7 @@
         <v>375</v>
       </c>
       <c r="H365" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="366" spans="1:8" x14ac:dyDescent="0.25">
@@ -6501,7 +6566,7 @@
         <v>376</v>
       </c>
       <c r="H366" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="367" spans="1:8" x14ac:dyDescent="0.25">
@@ -6512,7 +6577,7 @@
         <v>377</v>
       </c>
       <c r="H367" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="368" spans="1:8" x14ac:dyDescent="0.25">
@@ -6523,7 +6588,7 @@
         <v>378</v>
       </c>
       <c r="H368" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="369" spans="1:8" x14ac:dyDescent="0.25">
@@ -6534,7 +6599,7 @@
         <v>379</v>
       </c>
       <c r="H369" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="370" spans="1:8" x14ac:dyDescent="0.25">
@@ -6553,7 +6618,7 @@
         <v>380</v>
       </c>
       <c r="H371" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="372" spans="1:8" x14ac:dyDescent="0.25">
@@ -6564,7 +6629,7 @@
         <v>381</v>
       </c>
       <c r="H372" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="373" spans="1:8" x14ac:dyDescent="0.25">
@@ -6575,7 +6640,7 @@
         <v>382</v>
       </c>
       <c r="H373" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="374" spans="1:8" x14ac:dyDescent="0.25">
@@ -6586,7 +6651,7 @@
         <v>383</v>
       </c>
       <c r="H374" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="375" spans="1:8" x14ac:dyDescent="0.25">
@@ -6597,7 +6662,7 @@
         <v>384</v>
       </c>
       <c r="H375" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="376" spans="1:8" x14ac:dyDescent="0.25">
@@ -6608,7 +6673,7 @@
         <v>385</v>
       </c>
       <c r="H376" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="377" spans="1:8" x14ac:dyDescent="0.25">
@@ -6627,7 +6692,7 @@
       </c>
       <c r="D378" s="1"/>
       <c r="H378" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="379" spans="1:8" x14ac:dyDescent="0.25">
@@ -6641,7 +6706,7 @@
         <v>387</v>
       </c>
       <c r="H379" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="380" spans="1:8" x14ac:dyDescent="0.25">
@@ -6652,7 +6717,7 @@
         <v>388</v>
       </c>
       <c r="H380" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="381" spans="1:8" x14ac:dyDescent="0.25">
@@ -6660,7 +6725,7 @@
         <v>389</v>
       </c>
       <c r="H381" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="382" spans="1:8" x14ac:dyDescent="0.25">
@@ -6668,7 +6733,7 @@
         <v>390</v>
       </c>
       <c r="H382" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.25">
@@ -6676,7 +6741,7 @@
         <v>391</v>
       </c>
       <c r="H383" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="384" spans="1:8" x14ac:dyDescent="0.25">
@@ -6684,7 +6749,7 @@
         <v>392</v>
       </c>
       <c r="H384" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="385" spans="3:8" x14ac:dyDescent="0.25">
@@ -6692,7 +6757,7 @@
         <v>393</v>
       </c>
       <c r="H385" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="386" spans="3:8" x14ac:dyDescent="0.25">
@@ -6700,7 +6765,7 @@
         <v>394</v>
       </c>
       <c r="H386" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="387" spans="3:8" x14ac:dyDescent="0.25">
@@ -6708,7 +6773,7 @@
         <v>395</v>
       </c>
       <c r="H387" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="388" spans="3:8" x14ac:dyDescent="0.25">
@@ -6716,7 +6781,7 @@
         <v>396</v>
       </c>
       <c r="H388" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="389" spans="3:8" x14ac:dyDescent="0.25">
@@ -6724,7 +6789,7 @@
         <v>397</v>
       </c>
       <c r="H389" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="390" spans="3:8" x14ac:dyDescent="0.25">
@@ -6732,7 +6797,7 @@
         <v>398</v>
       </c>
       <c r="H390" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="391" spans="3:8" x14ac:dyDescent="0.25">
@@ -6740,7 +6805,7 @@
         <v>399</v>
       </c>
       <c r="H391" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>